<commit_message>
TAB-5581 Match small group spreadsheet locations against S+ list
</commit_message>
<xml_diff>
--- a/common/src/test/resources/sgt-import.xlsx
+++ b/common/src/test/resources/sgt-import.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17123"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/684a5dbc1ae6cefa/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alec/code/tabula/common/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27825" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="27820" windowHeight="11620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,15 @@
     <definedName name="Days">Lookups!$E$2:$E$8</definedName>
     <definedName name="SetTypes">Lookups!$A$2:$A$10</definedName>
   </definedNames>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="72">
   <si>
     <t>Module</t>
   </si>
@@ -245,13 +251,16 @@
   </si>
   <si>
     <t>Meeting</t>
+  </si>
+  <si>
+    <t>CS_CS1.04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,22 +618,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -682,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -729,14 +738,14 @@
       <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,7 +759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -761,7 +770,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -772,7 +781,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -783,7 +792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -794,7 +803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -805,7 +814,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -816,7 +825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -830,7 +839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -844,7 +853,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -858,7 +867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -881,26 +890,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="9.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -932,7 +941,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -961,7 +970,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -993,7 +1002,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1022,7 +1031,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1054,7 +1063,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1083,7 +1092,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1115,7 +1124,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1144,7 +1153,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1176,7 +1185,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1202,7 +1211,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1231,7 +1240,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1286,7 +1295,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1315,7 +1324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1344,7 +1353,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1373,7 +1382,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1399,7 +1408,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1421,14 +1430,14 @@
       <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -1439,7 +1448,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1450,7 +1459,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1461,7 +1470,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1472,7 +1481,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1480,7 +1489,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -1488,7 +1497,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -1496,7 +1505,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1504,12 +1513,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
TAB-5829 Add alt location diplay name field to SGT spreadsheet upload
</commit_message>
<xml_diff>
--- a/common/src/test/resources/sgt-import.xlsx
+++ b/common/src/test/resources/sgt-import.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="74">
   <si>
     <t>Module</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t>CS_CS1.04</t>
+  </si>
+  <si>
+    <t>Location display name</t>
+  </si>
+  <si>
+    <t>First-floor seminar room</t>
   </si>
 </sst>
 </file>
@@ -888,10 +894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -906,10 +912,11 @@
     <col min="8" max="8" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="2"/>
+    <col min="11" max="11" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -940,8 +947,11 @@
       <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -970,7 +980,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +1012,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1031,7 +1041,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1063,7 +1073,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1092,7 +1102,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1124,7 +1134,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1153,7 +1163,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1195,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1211,7 +1221,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1240,7 +1250,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1266,7 +1276,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1295,7 +1305,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1324,7 +1334,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1353,7 +1363,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1382,7 +1392,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1410,9 +1420,12 @@
       <c r="J17" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="K17" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G315">
       <formula1>Days</formula1>
     </dataValidation>

</xml_diff>